<commit_message>
Search (Test case) added
</commit_message>
<xml_diff>
--- a/src/test/java/Data/UserData.xlsx
+++ b/src/test/java/Data/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Automation(tarek)\Projects\AutomationPractice_Website\src\test\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24438433-6333-4754-A37B-1DAD8BE34FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4ABD1C-E2C5-4FB3-ACA0-3B9878199372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>Year</t>
   </si>
   <si>
-    <t>mostafa155744667@mostafa.com</t>
+    <t>mostafa1894667@mostafa.com</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>